<commit_message>
all the data ksharma12\fin_research\scripts\scripts\visualization_output
</commit_message>
<xml_diff>
--- a/scripts/scripts/realtime_output/multi_company_sep19/AUR_realtime_trades.xlsx
+++ b/scripts/scripts/realtime_output/multi_company_sep19/AUR_realtime_trades.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,22 +546,22 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45874.41702169457</v>
+        <v>45875.53912122138</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>3.14</v>
+        <v>3.2</v>
       </c>
       <c r="F2" t="n">
-        <v>3.078749346403958</v>
+        <v>3.094540909255746</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
       </c>
       <c r="H2" t="n">
-        <v>5.995</v>
+        <v>6.07</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -570,31 +570,283 @@
         <v>25</v>
       </c>
       <c r="K2" t="n">
-        <v>0.06125065359604243</v>
+        <v>0.1054590907442545</v>
       </c>
       <c r="L2" t="n">
         <v>100</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>45874.50162460537</v>
+        <v>45876.29025811746</v>
       </c>
       <c r="N2" t="n">
+        <v>6</v>
+      </c>
+      <c r="O2" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="P2" t="n">
+        <v>3.266588328671542</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AUR_14.0_Call</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45875.53912122138</v>
+      </c>
+      <c r="D3" t="n">
         <v>12</v>
       </c>
-      <c r="O2" t="n">
-        <v>3.14</v>
-      </c>
-      <c r="P2" t="n">
-        <v>3.165453023488038</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>2</v>
+      <c r="E3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.02877876720203026</v>
+      </c>
+      <c r="G3" t="n">
+        <v>14</v>
+      </c>
+      <c r="H3" t="n">
+        <v>6.07</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>25</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.02122123279796975</v>
+      </c>
+      <c r="L3" t="n">
+        <v>100</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>45876.4170691109</v>
+      </c>
+      <c r="N3" t="n">
+        <v>10</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.1517281683239983</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>AUR_3.0_Call</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45876.33251067522</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.123114092017505</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>25</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.07688590798249484</v>
+      </c>
+      <c r="L4" t="n">
+        <v>100</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>45876.4170691109</v>
+      </c>
+      <c r="N4" t="n">
+        <v>10</v>
+      </c>
+      <c r="O4" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="P4" t="n">
+        <v>3.20566315489788</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>AUR_11.0_Call</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45876.4593148956</v>
+      </c>
+      <c r="D5" t="n">
+        <v>11</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.03679925764654384</v>
+      </c>
+      <c r="G5" t="n">
+        <v>11</v>
+      </c>
+      <c r="H5" t="n">
+        <v>6.085</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>25</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.03320074235345617</v>
+      </c>
+      <c r="L5" t="n">
+        <v>100</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>45876.50165914217</v>
+      </c>
+      <c r="N5" t="n">
+        <v>12</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.08659202483859844</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>AUR_14.0_Call</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45876.4593148956</v>
+      </c>
+      <c r="D6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.005796167528757829</v>
+      </c>
+      <c r="G6" t="n">
+        <v>14</v>
+      </c>
+      <c r="H6" t="n">
+        <v>6.085</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>25</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.04420383247124218</v>
+      </c>
+      <c r="L6" t="n">
+        <v>100</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>45877.27325131699</v>
+      </c>
+      <c r="N6" t="n">
+        <v>6</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.09228680544472716</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>